<commit_message>
Update Paracosm Semester 2 Timetable.xlsx
</commit_message>
<xml_diff>
--- a/documents/Paracosm Semester 2 Timetable.xlsx
+++ b/documents/Paracosm Semester 2 Timetable.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\PARACOSM GIT\Paracosm\documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691298E5-7982-4819-9264-761AB8A35572}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="10695" yWindow="2220" windowWidth="16425" windowHeight="12000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Timeline</t>
   </si>
@@ -183,11 +192,6 @@
 Designing booth - decor, merch planning</t>
   </si>
   <si>
-    <t>marketing/sound - rhys
-unity functionality - cameron
-marketing and merch design - dana and hayley</t>
-  </si>
-  <si>
     <t>Playtest +  surveys
 Sound + music
 blog post</t>
@@ -291,14 +295,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -308,7 +313,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -342,47 +347,58 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -572,270 +588,1156 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47:F51"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="6" max="6" width="19.43"/>
+    <col min="6" max="6" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="6" t="s">
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="6" t="s">
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="6" t="s">
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="6" t="s">
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="6" t="s">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="6" t="s">
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J22" s="6" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="M22" s="6" t="s">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="6" t="s">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M27" s="6" t="s">
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+      <c r="M27" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="6" t="s">
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+    </row>
+    <row r="31" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="M32" s="6" t="s">
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="6" t="s">
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J37" s="6" t="s">
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M37" s="6" t="s">
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="6" t="s">
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="J42" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M42" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="6" t="s">
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="J47" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J47" s="6" t="s">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="M47" s="6" t="s">
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="J48" s="2"/>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
+      <c r="H49" s="2"/>
+      <c r="I49" s="2"/>
+      <c r="J49" s="2"/>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="J50" s="2"/>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+      <c r="M51" s="2"/>
+      <c r="N51" s="2"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="8" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="6" t="s">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G52" s="6" t="s">
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J52" s="6" t="s">
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+      <c r="M52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="M52" s="6" t="s">
+      <c r="N52" s="2"/>
+    </row>
+    <row r="53" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
+    </row>
+    <row r="55" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+      <c r="I55" s="2"/>
+      <c r="J55" s="2"/>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
+    </row>
+    <row r="56" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
+      <c r="J56" s="2"/>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
+      <c r="N56" s="2"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="6" t="s">
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="M57" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="G42:I46"/>
-    <mergeCell ref="J42:L46"/>
-    <mergeCell ref="A37:C41"/>
-    <mergeCell ref="D37:F41"/>
-    <mergeCell ref="G37:I41"/>
-    <mergeCell ref="J37:L41"/>
-    <mergeCell ref="M37:N41"/>
-    <mergeCell ref="D42:F46"/>
-    <mergeCell ref="M42:N46"/>
-    <mergeCell ref="D52:F56"/>
-    <mergeCell ref="G52:I56"/>
-    <mergeCell ref="A57:C61"/>
-    <mergeCell ref="D57:F61"/>
-    <mergeCell ref="G57:I61"/>
-    <mergeCell ref="J52:L56"/>
-    <mergeCell ref="M52:N56"/>
-    <mergeCell ref="J57:L61"/>
-    <mergeCell ref="M57:N61"/>
-    <mergeCell ref="A42:C46"/>
-    <mergeCell ref="A47:C51"/>
-    <mergeCell ref="D47:F51"/>
-    <mergeCell ref="G47:I51"/>
-    <mergeCell ref="J47:L51"/>
-    <mergeCell ref="M47:N51"/>
-    <mergeCell ref="A52:C56"/>
-    <mergeCell ref="G2:I6"/>
-    <mergeCell ref="J2:L6"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A22:C26"/>
+    <mergeCell ref="A27:C31"/>
+    <mergeCell ref="D27:F31"/>
+    <mergeCell ref="G27:I31"/>
+    <mergeCell ref="A32:C36"/>
+    <mergeCell ref="D32:F36"/>
+    <mergeCell ref="G32:I36"/>
+    <mergeCell ref="J12:L16"/>
+    <mergeCell ref="M12:N16"/>
+    <mergeCell ref="J17:L21"/>
+    <mergeCell ref="M17:N21"/>
+    <mergeCell ref="J22:L26"/>
+    <mergeCell ref="M22:N26"/>
+    <mergeCell ref="D22:F26"/>
+    <mergeCell ref="G22:I26"/>
+    <mergeCell ref="J27:L31"/>
+    <mergeCell ref="J32:L36"/>
+    <mergeCell ref="M32:N36"/>
+    <mergeCell ref="M27:N31"/>
+    <mergeCell ref="A12:C16"/>
+    <mergeCell ref="D12:F16"/>
+    <mergeCell ref="G12:I16"/>
+    <mergeCell ref="A17:C21"/>
+    <mergeCell ref="D17:F21"/>
+    <mergeCell ref="G17:I21"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="D2:F6"/>
     <mergeCell ref="M2:N6"/>
@@ -845,32 +1747,38 @@
     <mergeCell ref="G7:I11"/>
     <mergeCell ref="J7:L11"/>
     <mergeCell ref="M7:N11"/>
-    <mergeCell ref="A12:C16"/>
-    <mergeCell ref="D12:F16"/>
-    <mergeCell ref="G12:I16"/>
-    <mergeCell ref="A17:C21"/>
-    <mergeCell ref="D17:F21"/>
-    <mergeCell ref="G17:I21"/>
-    <mergeCell ref="D22:F26"/>
-    <mergeCell ref="G22:I26"/>
-    <mergeCell ref="J27:L31"/>
-    <mergeCell ref="J32:L36"/>
-    <mergeCell ref="M32:N36"/>
-    <mergeCell ref="J12:L16"/>
-    <mergeCell ref="M12:N16"/>
-    <mergeCell ref="J17:L21"/>
-    <mergeCell ref="M17:N21"/>
-    <mergeCell ref="J22:L26"/>
-    <mergeCell ref="M22:N26"/>
-    <mergeCell ref="M27:N31"/>
-    <mergeCell ref="A22:C26"/>
-    <mergeCell ref="A27:C31"/>
-    <mergeCell ref="D27:F31"/>
-    <mergeCell ref="G27:I31"/>
-    <mergeCell ref="A32:C36"/>
-    <mergeCell ref="D32:F36"/>
-    <mergeCell ref="G32:I36"/>
+    <mergeCell ref="G2:I6"/>
+    <mergeCell ref="J2:L6"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="A47:C51"/>
+    <mergeCell ref="D47:F51"/>
+    <mergeCell ref="G47:I51"/>
+    <mergeCell ref="J47:L51"/>
+    <mergeCell ref="M47:N51"/>
+    <mergeCell ref="A57:C61"/>
+    <mergeCell ref="D57:F61"/>
+    <mergeCell ref="G57:I61"/>
+    <mergeCell ref="J52:L56"/>
+    <mergeCell ref="M52:N56"/>
+    <mergeCell ref="J57:L61"/>
+    <mergeCell ref="M57:N61"/>
+    <mergeCell ref="A52:C56"/>
+    <mergeCell ref="M37:N41"/>
+    <mergeCell ref="D42:F46"/>
+    <mergeCell ref="M42:N46"/>
+    <mergeCell ref="D52:F56"/>
+    <mergeCell ref="G52:I56"/>
+    <mergeCell ref="G42:I46"/>
+    <mergeCell ref="J42:L46"/>
+    <mergeCell ref="A37:C41"/>
+    <mergeCell ref="D37:F41"/>
+    <mergeCell ref="G37:I41"/>
+    <mergeCell ref="J37:L41"/>
+    <mergeCell ref="A42:C46"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>